<commit_message>
adding algorithm vigenere and modified phpexcel libraries
</commit_message>
<xml_diff>
--- a/assets/excel/Data Kehadiran.xlsx
+++ b/assets/excel/Data Kehadiran.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Nama</t>
   </si>
@@ -26,28 +26,31 @@
     <t>Pulang</t>
   </si>
   <si>
-    <t>Anni Hapsah</t>
-  </si>
-  <si>
-    <t>2022-06-30 14:17:50</t>
-  </si>
-  <si>
-    <t>2022-06-30 13:39:14</t>
-  </si>
-  <si>
-    <t>2022-07-01 09:29:40</t>
-  </si>
-  <si>
-    <t>2022-06-30 13:44:22</t>
-  </si>
-  <si>
-    <t>2022-06-30 13:40:05</t>
-  </si>
-  <si>
-    <t>2022-06-30 13:40:26</t>
-  </si>
-  <si>
-    <t>2022-06-30 13:42:02</t>
+    <t>Bashir Rahadi</t>
+  </si>
+  <si>
+    <t>2022-07-04 20:42:33</t>
+  </si>
+  <si>
+    <t>2022-07-05 20:42:33</t>
+  </si>
+  <si>
+    <t>2022-07-07 09:39:59</t>
+  </si>
+  <si>
+    <t>2022-07-14 09:12:27</t>
+  </si>
+  <si>
+    <t>2022-07-14 09:12:53</t>
+  </si>
+  <si>
+    <t>2022-07-15 04:51:23</t>
+  </si>
+  <si>
+    <t>2022-07-15 08:31:03</t>
+  </si>
+  <si>
+    <t>2022-07-17 08:08:40</t>
   </si>
 </sst>
 </file>
@@ -386,7 +389,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -412,47 +415,65 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
+      <c r="C2"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C3"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4"/>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6"/>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>